<commit_message>
Change Self Evaluation Protocol
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Softuni\angularJs\Angular-Project-March-2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Issue-Tracking-System-AngularJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -371,10 +371,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -661,7 +661,7 @@
   <dimension ref="B2:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,11 +725,11 @@
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -748,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>16</v>
@@ -768,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="4">
         <v>20</v>
@@ -780,7 +780,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4">
         <v>30</v>
@@ -828,7 +828,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="C32" s="10">
         <f>SUM(C6:C31)</f>
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D32" s="10">
         <v>330</v>

</xml_diff>